<commit_message>
EasyController and EasyTelemetry almost ready to submit
</commit_message>
<xml_diff>
--- a/EasyController/BOM.xlsx
+++ b/EasyController/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A94C4F-090D-4E80-936F-6216142AE92C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3C42FA-74FF-4EBD-A98F-86CA0F5A3070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22257" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Digikey part #</t>
   </si>
@@ -45,18 +45,12 @@
     <t>Gate driver</t>
   </si>
   <si>
-    <t>497-6217-5-ND</t>
-  </si>
-  <si>
     <t>445-173257-1-ND</t>
   </si>
   <si>
     <t>1uF cap</t>
   </si>
   <si>
-    <t>296-47185-ND</t>
-  </si>
-  <si>
     <t>NFET</t>
   </si>
   <si>
@@ -66,12 +60,6 @@
     <t>TVS Diode</t>
   </si>
   <si>
-    <t>565-3998-ND</t>
-  </si>
-  <si>
-    <t>680uF cap</t>
-  </si>
-  <si>
     <t>CF14JT2K20CT-ND</t>
   </si>
   <si>
@@ -102,30 +90,12 @@
     <t>CF14JT47K0CT-ND</t>
   </si>
   <si>
-    <t>1050-1001-ND</t>
-  </si>
-  <si>
-    <t>Arduino Nano</t>
-  </si>
-  <si>
-    <t>S7013-ND</t>
-  </si>
-  <si>
-    <t>15 pin female header</t>
-  </si>
-  <si>
     <t>MCU1</t>
   </si>
   <si>
     <t>IC1</t>
   </si>
   <si>
-    <t>C1,C2,C3,C9,C11,C12,C13</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>IC2,IC3,IC4</t>
   </si>
   <si>
@@ -150,10 +120,67 @@
     <t>R1,R2,R3,R4,R5,R6</t>
   </si>
   <si>
-    <t>C6,C7,C8</t>
-  </si>
-  <si>
     <t>CF14JT22R0CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345-1092-ND‎ </t>
+  </si>
+  <si>
+    <t>Heatsink</t>
+  </si>
+  <si>
+    <t>Thermal paste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎1168-1380-ND‎ </t>
+  </si>
+  <si>
+    <t>497-6219-5-ND</t>
+  </si>
+  <si>
+    <t>497-1184-1-ND</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>5V Linear reg</t>
+  </si>
+  <si>
+    <t>1568-1231-ND</t>
+  </si>
+  <si>
+    <t>Teensy 3.2</t>
+  </si>
+  <si>
+    <t>14 pin male header</t>
+  </si>
+  <si>
+    <t>S1012EC-14-ND</t>
+  </si>
+  <si>
+    <t>S7012-ND</t>
+  </si>
+  <si>
+    <t>14 pin female header</t>
+  </si>
+  <si>
+    <t>R7,R8</t>
+  </si>
+  <si>
+    <t>C1,C2,C3,C11,C12,C13,C14</t>
+  </si>
+  <si>
+    <t>C6,C7,C8,C9</t>
+  </si>
+  <si>
+    <t>565-3994-ND</t>
+  </si>
+  <si>
+    <t>470uF cap</t>
+  </si>
+  <si>
+    <t>IRFB7730PBF-ND</t>
   </si>
 </sst>
 </file>
@@ -471,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,35 +529,35 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2">
-        <v>1.56</v>
+        <v>1.66</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="I2">
         <f>D2*C2</f>
-        <v>4.68</v>
+        <v>4.9799999999999995</v>
       </c>
       <c r="K2">
-        <f>SUM(I2:I100)</f>
-        <v>73.429999999999993</v>
+        <f>SUM(I2:I99)</f>
+        <v>68.369999999999976</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -539,40 +566,40 @@
         <v>0.33</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I18" si="0">D3*C3</f>
+        <f t="shared" ref="I3:I17" si="0">D3*C3</f>
         <v>2.31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>4.42</v>
+        <v>3.51</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>26.52</v>
+        <v>21.06</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -581,7 +608,7 @@
         <v>0.47</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -590,31 +617,31 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6">
-        <v>1.56</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>4.68</v>
+        <v>3.4499999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -623,7 +650,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -632,10 +659,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -644,7 +671,7 @@
         <v>0.16</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -653,10 +680,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -665,7 +692,7 @@
         <v>1.03</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -674,10 +701,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -686,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
@@ -695,10 +722,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -707,7 +734,7 @@
         <v>0.1</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
@@ -716,86 +743,123 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>0.98</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>1.96</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.1</v>
+        <v>0.35</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0.31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
       <c r="I15">
         <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0.91</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16">
+        <f>D16*C16</f>
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>